<commit_message>
done 4 tapi agak problem
</commit_message>
<xml_diff>
--- a/data_normalisasi.xlsx
+++ b/data_normalisasi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Tugas Kuliah\semester 4\kecerdasan buatan\program paper penentuan pilihan user\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1F74990-E77F-4791-8A29-A05959D6F93E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6BE48C9-C6C2-403F-9CDD-D5AF715BD8A7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7245" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,48 +35,6 @@
     <t>nama</t>
   </si>
   <si>
-    <t xml:space="preserve">1366 , 768  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1440 , 900  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1920 , 1080  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2560 , 1080  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3440 , 1440   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1920 , 1080   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">5120 , 1440  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1280 , 1024  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2560 , 1440   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3440 , 1440  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1600 , 900  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3840 , 2160   </t>
-  </si>
-  <si>
-    <t xml:space="preserve">3840 , 2160  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">2560 , 1440  </t>
-  </si>
-  <si>
     <t xml:space="preserve">LG 19M38A-B </t>
   </si>
   <si>
@@ -378,6 +336,48 @@
   </si>
   <si>
     <t xml:space="preserve">Samsung CF390 27-Inch </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1920x1080  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1366x768  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1440x900  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2560x1080  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3440x1440   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1920x1080   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5120x1440  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1280x1024  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2560x1440   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3440x1440  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1600x900  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3840x2160   </t>
+  </si>
+  <si>
+    <t xml:space="preserve">3840x2160  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">2560x1440  </t>
   </si>
 </sst>
 </file>
@@ -774,7 +774,7 @@
   <dimension ref="A1:D104"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A107" sqref="A107"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -801,7 +801,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>870000</v>
@@ -810,12 +810,12 @@
         <v>18.5</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>19</v>
+        <v>5</v>
       </c>
       <c r="B3">
         <v>669900</v>
@@ -824,12 +824,12 @@
         <v>19</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <v>1250000</v>
@@ -838,12 +838,12 @@
         <v>23.8</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>3015000</v>
@@ -852,12 +852,12 @@
         <v>30</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>5616000</v>
@@ -866,12 +866,12 @@
         <v>34</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="B7">
         <v>1799000</v>
@@ -880,12 +880,12 @@
         <v>27</v>
       </c>
       <c r="D7" t="s">
-        <v>6</v>
+        <v>105</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="B8">
         <v>1265000</v>
@@ -894,12 +894,12 @@
         <v>21.5</v>
       </c>
       <c r="D8" t="s">
-        <v>6</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="B9">
         <v>3359000</v>
@@ -908,12 +908,12 @@
         <v>23.8</v>
       </c>
       <c r="D9" t="s">
-        <v>9</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="B10">
         <v>1315000</v>
@@ -922,12 +922,12 @@
         <v>24</v>
       </c>
       <c r="D10" t="s">
-        <v>6</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="B11">
         <v>899000</v>
@@ -936,12 +936,12 @@
         <v>19</v>
       </c>
       <c r="D11" t="s">
-        <v>4</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="B12">
         <v>954000</v>
@@ -950,12 +950,12 @@
         <v>19.5</v>
       </c>
       <c r="D12" t="s">
-        <v>4</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="B13">
         <v>3215000</v>
@@ -964,12 +964,12 @@
         <v>29</v>
       </c>
       <c r="D13" t="s">
-        <v>7</v>
+        <v>108</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="B14">
         <v>1750000</v>
@@ -978,12 +978,12 @@
         <v>31.5</v>
       </c>
       <c r="D14" t="s">
-        <v>6</v>
+        <v>105</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
       <c r="B15">
         <v>1375000</v>
@@ -992,12 +992,12 @@
         <v>24</v>
       </c>
       <c r="D15" t="s">
-        <v>6</v>
+        <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="6" t="s">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B16">
         <v>1695000</v>
@@ -1006,12 +1006,12 @@
         <v>27</v>
       </c>
       <c r="D16" t="s">
-        <v>6</v>
+        <v>105</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
-        <v>33</v>
+        <v>19</v>
       </c>
       <c r="B17">
         <v>23550000</v>
@@ -1020,12 +1020,12 @@
         <v>49</v>
       </c>
       <c r="D17" t="s">
-        <v>10</v>
+        <v>111</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="B18">
         <v>3549900</v>
@@ -1034,12 +1034,12 @@
         <v>23.8</v>
       </c>
       <c r="D18" t="s">
-        <v>9</v>
+        <v>110</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="B19">
         <v>1545000</v>
@@ -1048,12 +1048,12 @@
         <v>24</v>
       </c>
       <c r="D19" t="s">
-        <v>9</v>
+        <v>110</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="6" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="B20">
         <v>3329000</v>
@@ -1062,12 +1062,12 @@
         <v>17</v>
       </c>
       <c r="D20" t="s">
-        <v>11</v>
+        <v>112</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="B21">
         <v>1230000</v>
@@ -1076,12 +1076,12 @@
         <v>23.8</v>
       </c>
       <c r="D21" t="s">
-        <v>6</v>
+        <v>105</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="B22">
         <v>1335000</v>
@@ -1090,12 +1090,12 @@
         <v>23.8</v>
       </c>
       <c r="D22" t="s">
-        <v>6</v>
+        <v>105</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="B23">
         <v>1900000</v>
@@ -1104,12 +1104,12 @@
         <v>18.5</v>
       </c>
       <c r="D23" t="s">
-        <v>4</v>
+        <v>106</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="6" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="B24">
         <v>1650000</v>
@@ -1118,12 +1118,12 @@
         <v>23.8</v>
       </c>
       <c r="D24" t="s">
-        <v>6</v>
+        <v>105</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="B25">
         <v>1235000</v>
@@ -1132,12 +1132,12 @@
         <v>21.5</v>
       </c>
       <c r="D25" t="s">
-        <v>6</v>
+        <v>105</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="B26">
         <v>4266000</v>
@@ -1146,12 +1146,12 @@
         <v>31.5</v>
       </c>
       <c r="D26" t="s">
-        <v>12</v>
+        <v>113</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="6" t="s">
-        <v>43</v>
+        <v>29</v>
       </c>
       <c r="B27">
         <v>1560000</v>
@@ -1160,12 +1160,12 @@
         <v>23.8</v>
       </c>
       <c r="D27" t="s">
-        <v>6</v>
+        <v>105</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>44</v>
+        <v>30</v>
       </c>
       <c r="B28">
         <v>5649000</v>
@@ -1174,12 +1174,12 @@
         <v>34</v>
       </c>
       <c r="D28" t="s">
-        <v>13</v>
+        <v>114</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="B29">
         <v>4750000</v>
@@ -1188,12 +1188,12 @@
         <v>27</v>
       </c>
       <c r="D29" t="s">
-        <v>6</v>
+        <v>105</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="B30">
         <v>1175000</v>
@@ -1202,12 +1202,12 @@
         <v>21.5</v>
       </c>
       <c r="D30" t="s">
-        <v>6</v>
+        <v>105</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
-        <v>47</v>
+        <v>33</v>
       </c>
       <c r="B31">
         <v>2368000</v>
@@ -1216,12 +1216,12 @@
         <v>23.8</v>
       </c>
       <c r="D31" t="s">
-        <v>6</v>
+        <v>105</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="B32">
         <v>600000</v>
@@ -1230,12 +1230,12 @@
         <v>19.5</v>
       </c>
       <c r="D32" t="s">
-        <v>14</v>
+        <v>115</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="B33">
         <v>3999000</v>
@@ -1244,12 +1244,12 @@
         <v>24</v>
       </c>
       <c r="D33" t="s">
-        <v>9</v>
+        <v>110</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="B34">
         <v>9550000</v>
@@ -1258,12 +1258,12 @@
         <v>27</v>
       </c>
       <c r="D34" t="s">
-        <v>15</v>
+        <v>116</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="B35">
         <v>1697000</v>
@@ -1272,12 +1272,12 @@
         <v>27</v>
       </c>
       <c r="D35" t="s">
-        <v>9</v>
+        <v>110</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="B36">
         <v>2388000</v>
@@ -1286,12 +1286,12 @@
         <v>27</v>
       </c>
       <c r="D36" t="s">
-        <v>9</v>
+        <v>110</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="B37">
         <v>3728000</v>
@@ -1300,12 +1300,12 @@
         <v>23.8</v>
       </c>
       <c r="D37" t="s">
-        <v>9</v>
+        <v>110</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="B38">
         <v>1029000</v>
@@ -1314,12 +1314,12 @@
         <v>19.5</v>
       </c>
       <c r="D38" t="s">
-        <v>6</v>
+        <v>105</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>55</v>
+        <v>41</v>
       </c>
       <c r="B39">
         <v>5499000</v>
@@ -1328,12 +1328,12 @@
         <v>27</v>
       </c>
       <c r="D39" t="s">
-        <v>16</v>
+        <v>117</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="6" t="s">
-        <v>56</v>
+        <v>42</v>
       </c>
       <c r="B40">
         <v>1999000</v>
@@ -1342,12 +1342,12 @@
         <v>19.5</v>
       </c>
       <c r="D40" t="s">
-        <v>14</v>
+        <v>115</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="B41">
         <v>3700000</v>
@@ -1356,12 +1356,12 @@
         <v>27</v>
       </c>
       <c r="D41" t="s">
-        <v>12</v>
+        <v>113</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="B42">
         <v>1000000</v>
@@ -1370,12 +1370,12 @@
         <v>24</v>
       </c>
       <c r="D42" t="s">
-        <v>6</v>
+        <v>105</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="B43">
         <v>1170000</v>
@@ -1384,12 +1384,12 @@
         <v>19.5</v>
       </c>
       <c r="D43" t="s">
-        <v>14</v>
+        <v>115</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="B44">
         <v>3207000</v>
@@ -1398,12 +1398,12 @@
         <v>27</v>
       </c>
       <c r="D44" t="s">
-        <v>6</v>
+        <v>105</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="B45">
         <v>1682500</v>
@@ -1412,12 +1412,12 @@
         <v>17</v>
       </c>
       <c r="D45" t="s">
-        <v>11</v>
+        <v>112</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
       <c r="B46">
         <v>5686000</v>
@@ -1426,12 +1426,12 @@
         <v>27</v>
       </c>
       <c r="D46" t="s">
-        <v>12</v>
+        <v>113</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
-        <v>63</v>
+        <v>49</v>
       </c>
       <c r="B47">
         <v>4650000</v>
@@ -1440,12 +1440,12 @@
         <v>24.5</v>
       </c>
       <c r="D47" t="s">
-        <v>6</v>
+        <v>105</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="6" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="B48">
         <v>1285000</v>
@@ -1454,12 +1454,12 @@
         <v>21.5</v>
       </c>
       <c r="D48" t="s">
-        <v>6</v>
+        <v>105</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="6" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="B49">
         <v>952000</v>
@@ -1468,12 +1468,12 @@
         <v>21.5</v>
       </c>
       <c r="D49" t="s">
-        <v>6</v>
+        <v>105</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="6" t="s">
-        <v>66</v>
+        <v>52</v>
       </c>
       <c r="B50">
         <v>1278000</v>
@@ -1482,12 +1482,12 @@
         <v>27</v>
       </c>
       <c r="D50" t="s">
-        <v>6</v>
+        <v>105</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
-        <v>67</v>
+        <v>53</v>
       </c>
       <c r="B51">
         <v>2450000</v>
@@ -1496,12 +1496,12 @@
         <v>21.5</v>
       </c>
       <c r="D51" t="s">
-        <v>6</v>
+        <v>105</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="B52">
         <v>1060000</v>
@@ -1510,12 +1510,12 @@
         <v>19.5</v>
       </c>
       <c r="D52" t="s">
-        <v>14</v>
+        <v>115</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="B53">
         <v>1319000</v>
@@ -1524,12 +1524,12 @@
         <v>24</v>
       </c>
       <c r="D53" t="s">
-        <v>6</v>
+        <v>105</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="6" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="B54">
         <v>992000</v>
@@ -1538,12 +1538,12 @@
         <v>18.5</v>
       </c>
       <c r="D54" t="s">
-        <v>4</v>
+        <v>106</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="6" t="s">
-        <v>71</v>
+        <v>57</v>
       </c>
       <c r="B55">
         <v>1600000</v>
@@ -1552,12 +1552,12 @@
         <v>23.6</v>
       </c>
       <c r="D55" t="s">
-        <v>4</v>
+        <v>106</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="6" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="B56">
         <v>2597000</v>
@@ -1566,12 +1566,12 @@
         <v>23.8</v>
       </c>
       <c r="D56" t="s">
-        <v>6</v>
+        <v>105</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="6" t="s">
-        <v>73</v>
+        <v>59</v>
       </c>
       <c r="B57">
         <v>1500000</v>
@@ -1580,12 +1580,12 @@
         <v>21.5</v>
       </c>
       <c r="D57" t="s">
-        <v>6</v>
+        <v>105</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="6" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="B58">
         <v>1725000</v>
@@ -1594,12 +1594,12 @@
         <v>18.5</v>
       </c>
       <c r="D58" t="s">
-        <v>4</v>
+        <v>106</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="6" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="B59">
         <v>1150000</v>
@@ -1608,12 +1608,12 @@
         <v>18.5</v>
       </c>
       <c r="D59" t="s">
-        <v>4</v>
+        <v>106</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="6" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="B60">
         <v>1825000</v>
@@ -1622,12 +1622,12 @@
         <v>23.8</v>
       </c>
       <c r="D60" t="s">
-        <v>6</v>
+        <v>105</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="6" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="B61">
         <v>1849000</v>
@@ -1636,12 +1636,12 @@
         <v>18.5</v>
       </c>
       <c r="D61" t="s">
-        <v>4</v>
+        <v>106</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="6" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="B62">
         <v>595000</v>
@@ -1650,12 +1650,12 @@
         <v>20</v>
       </c>
       <c r="D62" t="s">
-        <v>14</v>
+        <v>115</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="B63">
         <v>1480000</v>
@@ -1664,12 +1664,12 @@
         <v>24</v>
       </c>
       <c r="D63" t="s">
-        <v>6</v>
+        <v>105</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="6" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="B64">
         <v>2690000</v>
@@ -1678,12 +1678,12 @@
         <v>25</v>
       </c>
       <c r="D64" t="s">
-        <v>7</v>
+        <v>108</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="6" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="B65">
         <v>2425000</v>
@@ -1692,12 +1692,12 @@
         <v>21.5</v>
       </c>
       <c r="D65" t="s">
-        <v>6</v>
+        <v>105</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="6" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="B66">
         <v>1250000</v>
@@ -1706,12 +1706,12 @@
         <v>21.5</v>
       </c>
       <c r="D66" t="s">
-        <v>6</v>
+        <v>105</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
-        <v>83</v>
+        <v>69</v>
       </c>
       <c r="B67">
         <v>6890000</v>
@@ -1720,12 +1720,12 @@
         <v>27</v>
       </c>
       <c r="D67" t="s">
-        <v>17</v>
+        <v>118</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="6" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="B68">
         <v>873000</v>
@@ -1734,12 +1734,12 @@
         <v>18.5</v>
       </c>
       <c r="D68" t="s">
-        <v>4</v>
+        <v>106</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="6" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="B69">
         <v>650000</v>
@@ -1748,12 +1748,12 @@
         <v>19.5</v>
       </c>
       <c r="D69" t="s">
-        <v>5</v>
+        <v>107</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="6" t="s">
-        <v>86</v>
+        <v>72</v>
       </c>
       <c r="B70">
         <v>5735000</v>
@@ -1762,12 +1762,12 @@
         <v>32</v>
       </c>
       <c r="D70" t="s">
-        <v>12</v>
+        <v>113</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="6" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="B71">
         <v>4699000</v>
@@ -1776,12 +1776,12 @@
         <v>19</v>
       </c>
       <c r="D71" t="s">
-        <v>11</v>
+        <v>112</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="6" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="B72">
         <v>3822000</v>
@@ -1790,12 +1790,12 @@
         <v>19</v>
       </c>
       <c r="D72" t="s">
-        <v>4</v>
+        <v>106</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="6" t="s">
-        <v>89</v>
+        <v>75</v>
       </c>
       <c r="B73">
         <v>5850000</v>
@@ -1804,12 +1804,12 @@
         <v>23.8</v>
       </c>
       <c r="D73" t="s">
-        <v>6</v>
+        <v>105</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="6" t="s">
-        <v>90</v>
+        <v>76</v>
       </c>
       <c r="B74">
         <v>10111000</v>
@@ -1818,12 +1818,12 @@
         <v>27</v>
       </c>
       <c r="D74" t="s">
-        <v>6</v>
+        <v>105</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="6" t="s">
-        <v>91</v>
+        <v>77</v>
       </c>
       <c r="B75">
         <v>16685000</v>
@@ -1832,12 +1832,12 @@
         <v>26.9</v>
       </c>
       <c r="D75" t="s">
-        <v>17</v>
+        <v>118</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="6" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="B76">
         <v>8939000</v>
@@ -1846,12 +1846,12 @@
         <v>23.8</v>
       </c>
       <c r="D76" t="s">
-        <v>6</v>
+        <v>105</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="6" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="B77">
         <v>18999000</v>
@@ -1860,12 +1860,12 @@
         <v>25</v>
       </c>
       <c r="D77" t="s">
-        <v>6</v>
+        <v>105</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="6" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="B78">
         <v>4675000</v>
@@ -1874,12 +1874,12 @@
         <v>23.8</v>
       </c>
       <c r="D78" t="s">
-        <v>6</v>
+        <v>105</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="6" t="s">
-        <v>95</v>
+        <v>81</v>
       </c>
       <c r="B79">
         <v>988000</v>
@@ -1888,12 +1888,12 @@
         <v>19.5</v>
       </c>
       <c r="D79" t="s">
-        <v>14</v>
+        <v>115</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="6" t="s">
-        <v>96</v>
+        <v>82</v>
       </c>
       <c r="B80">
         <v>10426000</v>
@@ -1902,12 +1902,12 @@
         <v>27</v>
       </c>
       <c r="D80" t="s">
-        <v>16</v>
+        <v>117</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="6" t="s">
-        <v>97</v>
+        <v>83</v>
       </c>
       <c r="B81">
         <v>15999000</v>
@@ -1916,12 +1916,12 @@
         <v>32</v>
       </c>
       <c r="D81" t="s">
-        <v>17</v>
+        <v>118</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="6" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="B82">
         <v>8748000</v>
@@ -1930,12 +1930,12 @@
         <v>23.8</v>
       </c>
       <c r="D82" t="s">
-        <v>6</v>
+        <v>105</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="6" t="s">
-        <v>99</v>
+        <v>85</v>
       </c>
       <c r="B83">
         <v>2899000</v>
@@ -1944,12 +1944,12 @@
         <v>21.5</v>
       </c>
       <c r="D83" t="s">
-        <v>6</v>
+        <v>105</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="6" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="B84">
         <v>5083000</v>
@@ -1958,12 +1958,12 @@
         <v>24</v>
       </c>
       <c r="D84" t="s">
-        <v>6</v>
+        <v>105</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="6" t="s">
-        <v>101</v>
+        <v>87</v>
       </c>
       <c r="B85">
         <v>2719900</v>
@@ -1972,12 +1972,12 @@
         <v>21.5</v>
       </c>
       <c r="D85" t="s">
-        <v>6</v>
+        <v>105</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="6" t="s">
-        <v>102</v>
+        <v>88</v>
       </c>
       <c r="B86">
         <v>78210000</v>
@@ -1986,12 +1986,12 @@
         <v>65</v>
       </c>
       <c r="D86" t="s">
-        <v>15</v>
+        <v>116</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="6" t="s">
-        <v>103</v>
+        <v>89</v>
       </c>
       <c r="B87">
         <v>59577208</v>
@@ -2000,12 +2000,12 @@
         <v>24</v>
       </c>
       <c r="D87" t="s">
-        <v>9</v>
+        <v>110</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="6" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
       <c r="B88">
         <v>15808000</v>
@@ -2014,12 +2014,12 @@
         <v>27</v>
       </c>
       <c r="D88" t="s">
-        <v>16</v>
+        <v>117</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="6" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
       <c r="B89">
         <v>19028000</v>
@@ -2028,12 +2028,12 @@
         <v>32</v>
       </c>
       <c r="D89" t="s">
-        <v>16</v>
+        <v>117</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="6" t="s">
-        <v>106</v>
+        <v>92</v>
       </c>
       <c r="B90">
         <v>3662010</v>
@@ -2042,12 +2042,12 @@
         <v>23.8</v>
       </c>
       <c r="D90" t="s">
-        <v>6</v>
+        <v>105</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="6" t="s">
-        <v>107</v>
+        <v>93</v>
       </c>
       <c r="B91">
         <v>3510000</v>
@@ -2056,12 +2056,12 @@
         <v>23.8</v>
       </c>
       <c r="D91" t="s">
-        <v>6</v>
+        <v>105</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="6" t="s">
-        <v>108</v>
+        <v>94</v>
       </c>
       <c r="B92">
         <v>4218800</v>
@@ -2070,12 +2070,12 @@
         <v>21.5</v>
       </c>
       <c r="D92" t="s">
-        <v>6</v>
+        <v>105</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="6" t="s">
-        <v>109</v>
+        <v>95</v>
       </c>
       <c r="B93">
         <v>11328000</v>
@@ -2084,12 +2084,12 @@
         <v>15.6</v>
       </c>
       <c r="D93" t="s">
-        <v>6</v>
+        <v>105</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="6" t="s">
-        <v>110</v>
+        <v>96</v>
       </c>
       <c r="B94">
         <v>4550000</v>
@@ -2098,12 +2098,12 @@
         <v>24</v>
       </c>
       <c r="D94" t="s">
-        <v>6</v>
+        <v>105</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="6" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="B95">
         <v>12402000</v>
@@ -2112,12 +2112,12 @@
         <v>27</v>
       </c>
       <c r="D95" t="s">
-        <v>17</v>
+        <v>118</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="6" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="B96">
         <v>4512000</v>
@@ -2126,12 +2126,12 @@
         <v>23.8</v>
       </c>
       <c r="D96" t="s">
-        <v>6</v>
+        <v>105</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="6" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="B97">
         <v>12100000</v>
@@ -2140,12 +2140,12 @@
         <v>31.5</v>
       </c>
       <c r="D97" t="s">
-        <v>17</v>
+        <v>118</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="6" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="B98">
         <v>3228900</v>
@@ -2154,12 +2154,12 @@
         <v>21.5</v>
       </c>
       <c r="D98" t="s">
-        <v>6</v>
+        <v>105</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="6" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="B99">
         <v>15421000</v>
@@ -2168,12 +2168,12 @@
         <v>24</v>
       </c>
       <c r="D99" t="s">
-        <v>6</v>
+        <v>105</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="6" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="B100">
         <v>6552810</v>
@@ -2182,12 +2182,12 @@
         <v>27</v>
       </c>
       <c r="D100" t="s">
-        <v>6</v>
+        <v>105</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="6" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="B101">
         <v>11570000</v>
@@ -2196,12 +2196,12 @@
         <v>24</v>
       </c>
       <c r="D101" t="s">
-        <v>6</v>
+        <v>105</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="6" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="B102">
         <v>4369950</v>
@@ -2210,7 +2210,7 @@
         <v>27</v>
       </c>
       <c r="D102" t="s">
-        <v>6</v>
+        <v>105</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>